<commit_message>
add script to mass import consultants
</commit_message>
<xml_diff>
--- a/_data_test/hr.presence-2.xlsx
+++ b/_data_test/hr.presence-2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">VALUED</t>
   </si>
   <si>
+    <t xml:space="preserve">LEAVE</t>
+  </si>
+  <si>
     <t xml:space="preserve">PARTIAL_TIME</t>
   </si>
   <si>
@@ -52,12 +55,15 @@
     <t xml:space="preserve">GRADE</t>
   </si>
   <si>
-    <t xml:space="preserve">CDM</t>
+    <t xml:space="preserve">IS_CDM</t>
   </si>
   <si>
     <t xml:space="preserve">CDM_MATRICULE</t>
   </si>
   <si>
+    <t xml:space="preserve">CDM_NAME</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prénom NOM 1</t>
   </si>
   <si>
@@ -76,7 +82,7 @@
     <t xml:space="preserve">Consultant</t>
   </si>
   <si>
-    <t xml:space="preserve">Victoire PERRIN</t>
+    <t xml:space="preserve">false</t>
   </si>
   <si>
     <t xml:space="preserve">3707</t>
@@ -112,9 +118,6 @@
     <t xml:space="preserve">Analyst</t>
   </si>
   <si>
-    <t xml:space="preserve">5267</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prénom NOM 5</t>
   </si>
   <si>
@@ -167,6 +170,21 @@
   </si>
   <si>
     <t xml:space="preserve">000008488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prénom NOM 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prenom-nom-11@mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000003707</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senior Consultant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
   </si>
 </sst>
 </file>
@@ -251,7 +269,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,6 +284,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -285,16 +307,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="0" width="30.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="16.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,19 +365,25 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>42737</v>
@@ -354,37 +391,38 @@
       <c r="F2" s="3" t="n">
         <v>43556</v>
       </c>
-      <c r="G2" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G2" s="3"/>
       <c r="H2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
+      <c r="I2" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>43102</v>
@@ -392,37 +430,38 @@
       <c r="F3" s="3" t="n">
         <v>43102</v>
       </c>
-      <c r="G3" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>16</v>
+      <c r="I3" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>42996</v>
@@ -430,37 +469,38 @@
       <c r="F4" s="3" t="n">
         <v>42996</v>
       </c>
-      <c r="G4" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G4" s="3"/>
       <c r="H4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>16</v>
+      <c r="I4" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>43899</v>
@@ -468,75 +508,79 @@
       <c r="F5" s="3" t="n">
         <v>43899</v>
       </c>
-      <c r="G5" s="2" t="n">
-        <v>1</v>
+      <c r="G5" s="3" t="n">
+        <v>44255</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>16</v>
+      <c r="I5" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>43073</v>
+        <v>44290</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>43073</v>
       </c>
-      <c r="G6" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>16</v>
+      <c r="I6" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>42989</v>
@@ -544,37 +588,38 @@
       <c r="F7" s="3" t="n">
         <v>42989</v>
       </c>
-      <c r="G7" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>16</v>
+      <c r="I7" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>43017</v>
@@ -582,37 +627,38 @@
       <c r="F8" s="3" t="n">
         <v>43017</v>
       </c>
-      <c r="G8" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G8" s="3"/>
       <c r="H8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>16</v>
+      <c r="I8" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>43678</v>
@@ -620,37 +666,38 @@
       <c r="F9" s="3" t="n">
         <v>43678</v>
       </c>
-      <c r="G9" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G9" s="3"/>
       <c r="H9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>16</v>
+      <c r="I9" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>43374</v>
@@ -658,37 +705,38 @@
       <c r="F10" s="3" t="n">
         <v>43374</v>
       </c>
-      <c r="G10" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>16</v>
+      <c r="I10" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>43045</v>
@@ -696,23 +744,59 @@
       <c r="F11" s="3" t="n">
         <v>43045</v>
       </c>
-      <c r="G11" s="2" t="n">
-        <v>1</v>
-      </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>16</v>
+      <c r="I11" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>41603</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>41603</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -726,6 +810,7 @@
     <hyperlink ref="B9" r:id="rId7" display="prenom-nom-8@mail.com"/>
     <hyperlink ref="B10" r:id="rId8" display="prenom-nom-9@mail.com"/>
     <hyperlink ref="B11" r:id="rId9" display="prenom-nom-10@mail.com"/>
+    <hyperlink ref="B12" r:id="rId10" display="prenom-nom-11@mail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
add import to update pxx
</commit_message>
<xml_diff>
--- a/_data_test/hr.presence-2.xlsx
+++ b/_data_test/hr.presence-2.xlsx
@@ -310,7 +310,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -544,7 +544,7 @@
         <v>34</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>44290</v>
+        <v>44259</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>43073</v>

</xml_diff>

<commit_message>
add recalcul Pxx after import of consultant profil
</commit_message>
<xml_diff>
--- a/_data_test/hr.presence-2.xlsx
+++ b/_data_test/hr.presence-2.xlsx
@@ -309,11 +309,11 @@
   </sheetPr>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.09"/>
@@ -544,7 +544,7 @@
         <v>34</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>44259</v>
+        <v>44320</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>43073</v>

</xml_diff>